<commit_message>
Removed broken UNICODE in Kettle scripts.
</commit_message>
<xml_diff>
--- a/GazetteerETL/GeoData/AdHoc/AdHoc.xlsx
+++ b/GazetteerETL/GeoData/AdHoc/AdHoc.xlsx
@@ -1262,9 +1262,6 @@
     <t/>
   </si>
   <si>
-    <t>NGA GEONAMES</t>
-  </si>
-  <si>
     <t>NGA-784547</t>
   </si>
   <si>
@@ -1364,9 +1361,6 @@
     <t>Gaza</t>
   </si>
   <si>
-    <t>USGS GNIS</t>
-  </si>
-  <si>
     <t>Jersey</t>
   </si>
   <si>
@@ -1422,6 +1416,12 @@
   </si>
   <si>
     <t>US State Code</t>
+  </si>
+  <si>
+    <t>NGA</t>
+  </si>
+  <si>
+    <t>USGS</t>
   </si>
 </sst>
 </file>
@@ -2270,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,10 +2346,10 @@
         <v>1</v>
       </c>
       <c r="R1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2677,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C10" s="2">
         <v>39.76</v>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -2732,7 +2732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2807,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S2" s="2"/>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S3" s="2"/>
     </row>
@@ -2952,7 +2952,7 @@
         <v>1779780</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>1779781</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>294478</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
         <v>1779783</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>1779784</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>448508</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
         <v>1779785</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>481813</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
         <v>481813</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S12" s="2"/>
     </row>
@@ -3349,7 +3349,7 @@
         <v>1779787</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S13" s="2"/>
     </row>
@@ -3394,7 +3394,7 @@
         <v>662849</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S14" s="2"/>
     </row>
@@ -3439,7 +3439,7 @@
         <v>1779793</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S15" s="2"/>
     </row>
@@ -3484,7 +3484,7 @@
         <v>1779796</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S16" s="2"/>
     </row>
@@ -3529,7 +3529,7 @@
         <v>1085497</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S17" s="2"/>
     </row>
@@ -3574,7 +3574,7 @@
         <v>1102857</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S18" s="2"/>
     </row>
@@ -3619,7 +3619,7 @@
         <v>1155107</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S19" s="2"/>
     </row>
@@ -3664,7 +3664,7 @@
         <v>1325873</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S20" s="2"/>
     </row>
@@ -3709,7 +3709,7 @@
         <v>1779801</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S21" s="2"/>
     </row>
@@ -3754,7 +3754,7 @@
         <v>1455989</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S22" s="2"/>
     </row>
@@ -3799,7 +3799,7 @@
         <v>1779804</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S23" s="2"/>
     </row>
@@ -3844,7 +3844,7 @@
         <v>1779804</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S24" s="2"/>
     </row>
@@ -3889,7 +3889,7 @@
         <v>1779805</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S25" s="2"/>
     </row>
@@ -3934,7 +3934,7 @@
         <v>1779806</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S26" s="2"/>
     </row>
@@ -3979,7 +3979,7 @@
         <v>1779807</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S27" s="2"/>
     </row>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S28" s="3"/>
     </row>
@@ -4073,7 +4073,7 @@
         <v>68085</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S29" s="2"/>
     </row>
@@ -4118,7 +4118,7 @@
         <v>1779778</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S30" s="2"/>
     </row>
@@ -4163,7 +4163,7 @@
         <v>1779779</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S31" s="2"/>
     </row>
@@ -4208,7 +4208,7 @@
         <v>1779781</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4252,7 +4252,7 @@
         <v>1702382</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -4296,7 +4296,7 @@
         <v>294478</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S34" s="2"/>
     </row>
@@ -4341,7 +4341,7 @@
         <v>1779782</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S35" s="2"/>
     </row>
@@ -4386,7 +4386,7 @@
         <v>1779783</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S36" s="2"/>
     </row>
@@ -4431,7 +4431,7 @@
         <v>1779784</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -4475,7 +4475,7 @@
         <v>448508</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S38" s="2"/>
     </row>
@@ -4520,7 +4520,7 @@
         <v>1779785</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S39" s="2"/>
     </row>
@@ -4565,7 +4565,7 @@
         <v>481813</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S40" s="2"/>
     </row>
@@ -4610,7 +4610,7 @@
         <v>1779786</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -4654,7 +4654,7 @@
         <v>1779792</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S42" s="2"/>
     </row>
@@ -4699,7 +4699,7 @@
         <v>1779793</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S43" s="2"/>
     </row>
@@ -4744,7 +4744,7 @@
         <v>1779794</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S44" s="2"/>
     </row>
@@ -4789,7 +4789,7 @@
         <v>1779795</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S45" s="2"/>
     </row>
@@ -4834,7 +4834,7 @@
         <v>897535</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S46" s="2"/>
     </row>
@@ -4879,7 +4879,7 @@
         <v>1779796</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S47" s="2"/>
     </row>
@@ -4924,7 +4924,7 @@
         <v>1027616</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S48" s="2"/>
     </row>
@@ -4969,7 +4969,7 @@
         <v>1779797</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S49" s="2"/>
     </row>
@@ -5014,7 +5014,7 @@
         <v>1155107</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S50" s="2"/>
     </row>
@@ -5059,7 +5059,7 @@
         <v>1219835</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S51" s="2"/>
     </row>
@@ -5104,7 +5104,7 @@
         <v>1779799</v>
       </c>
       <c r="R52" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S52" s="2"/>
     </row>
@@ -5149,7 +5149,7 @@
         <v>1785534</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -5193,7 +5193,7 @@
         <v>1779801</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -5237,7 +5237,7 @@
         <v>1779805</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -5281,7 +5281,7 @@
         <v>1779806</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -5325,7 +5325,7 @@
         <v>1779807</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -5369,7 +5369,7 @@
         <v>1785533</v>
       </c>
       <c r="R58" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -5413,7 +5413,7 @@
         <v>1779777</v>
       </c>
       <c r="R59" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -5457,7 +5457,7 @@
         <v>1779778</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5501,7 +5501,7 @@
         <v>1779779</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -5545,7 +5545,7 @@
         <v>1779780</v>
       </c>
       <c r="R62" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -5589,7 +5589,7 @@
         <v>294478</v>
       </c>
       <c r="R63" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -5633,7 +5633,7 @@
         <v>1779784</v>
       </c>
       <c r="R64" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -5677,7 +5677,7 @@
         <v>481813</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -5721,7 +5721,7 @@
         <v>1779786</v>
       </c>
       <c r="R66" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -5765,7 +5765,7 @@
         <v>606926</v>
       </c>
       <c r="R67" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -5809,7 +5809,7 @@
         <v>1779789</v>
       </c>
       <c r="R68" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -5853,7 +5853,7 @@
         <v>662849</v>
       </c>
       <c r="R69" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -5897,7 +5897,7 @@
         <v>1779790</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -5941,7 +5941,7 @@
         <v>767982</v>
       </c>
       <c r="R71" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -5985,7 +5985,7 @@
         <v>1779792</v>
       </c>
       <c r="R72" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -6029,7 +6029,7 @@
         <v>1102857</v>
       </c>
       <c r="R73" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -6073,7 +6073,7 @@
         <v>1155107</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="75" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6117,7 +6117,7 @@
         <v>1779798</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -6161,7 +6161,7 @@
         <v>1325873</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -6205,7 +6205,7 @@
         <v>1779803</v>
       </c>
       <c r="R77" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -6249,7 +6249,7 @@
         <v>1779804</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="Q79" s="2"/>
       <c r="R79" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S79" s="2"/>
     </row>
@@ -6342,7 +6342,7 @@
         <v>1779806</v>
       </c>
       <c r="R80" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
@@ -6386,7 +6386,7 @@
         <v>1779778</v>
       </c>
       <c r="R81" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
@@ -6430,7 +6430,7 @@
         <v>897535</v>
       </c>
       <c r="R82" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -6474,7 +6474,7 @@
         <v>1779798</v>
       </c>
       <c r="R83" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
@@ -6518,7 +6518,7 @@
         <v>1779805</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -6562,7 +6562,7 @@
         <v>897535</v>
       </c>
       <c r="R85" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
@@ -6606,7 +6606,7 @@
         <v>1027616</v>
       </c>
       <c r="R86" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
@@ -6650,7 +6650,7 @@
         <v>1779797</v>
       </c>
       <c r="R87" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -6694,7 +6694,7 @@
         <v>1779799</v>
       </c>
       <c r="R88" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -6738,7 +6738,7 @@
         <v>1785534</v>
       </c>
       <c r="R89" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -6782,7 +6782,7 @@
         <v>1779805</v>
       </c>
       <c r="R90" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -6826,7 +6826,7 @@
         <v>1702382</v>
       </c>
       <c r="R91" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -6870,7 +6870,7 @@
         <v>1702382</v>
       </c>
       <c r="R92" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -6914,7 +6914,7 @@
         <v>1219835</v>
       </c>
       <c r="R93" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -6962,10 +6962,10 @@
       </c>
       <c r="Q94" s="3"/>
       <c r="R94" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S94" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -7009,10 +7009,10 @@
         <v>1785533</v>
       </c>
       <c r="R95" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S95" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -7056,10 +7056,10 @@
         <v>1779777</v>
       </c>
       <c r="R96" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S96" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -7103,10 +7103,10 @@
         <v>68085</v>
       </c>
       <c r="R97" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S97" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -7150,10 +7150,10 @@
         <v>1779778</v>
       </c>
       <c r="R98" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S98" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7197,10 +7197,10 @@
         <v>1779779</v>
       </c>
       <c r="R99" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S99" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7244,10 +7244,10 @@
         <v>1779780</v>
       </c>
       <c r="R100" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7291,10 +7291,10 @@
         <v>1779781</v>
       </c>
       <c r="R101" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S101" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
@@ -7338,10 +7338,10 @@
         <v>1702382</v>
       </c>
       <c r="R102" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S102" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
@@ -7385,10 +7385,10 @@
         <v>294478</v>
       </c>
       <c r="R103" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S103" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -7432,10 +7432,10 @@
         <v>1705317</v>
       </c>
       <c r="R104" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S104" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
@@ -7479,10 +7479,10 @@
         <v>1779782</v>
       </c>
       <c r="R105" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S105" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
@@ -7526,10 +7526,10 @@
         <v>1779783</v>
       </c>
       <c r="R106" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S106" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
@@ -7573,10 +7573,10 @@
         <v>1779784</v>
       </c>
       <c r="R107" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S107" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
@@ -7620,10 +7620,10 @@
         <v>448508</v>
       </c>
       <c r="R108" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
@@ -7667,10 +7667,10 @@
         <v>1779785</v>
       </c>
       <c r="R109" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S109" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
@@ -7714,10 +7714,10 @@
         <v>481813</v>
       </c>
       <c r="R110" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
@@ -7761,10 +7761,10 @@
         <v>1779786</v>
       </c>
       <c r="R111" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S111" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
@@ -7808,10 +7808,10 @@
         <v>1629543</v>
       </c>
       <c r="R112" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -7855,10 +7855,10 @@
         <v>1779787</v>
       </c>
       <c r="R113" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S113" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -7902,10 +7902,10 @@
         <v>1714934</v>
       </c>
       <c r="R114" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
@@ -7949,10 +7949,10 @@
         <v>606926</v>
       </c>
       <c r="R115" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -7996,10 +7996,10 @@
         <v>1779789</v>
       </c>
       <c r="R116" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
@@ -8043,10 +8043,10 @@
         <v>662849</v>
       </c>
       <c r="R117" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S117" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
@@ -8090,10 +8090,10 @@
         <v>1779790</v>
       </c>
       <c r="R118" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S118" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
@@ -8137,10 +8137,10 @@
         <v>1779791</v>
       </c>
       <c r="R119" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S119" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
@@ -8184,10 +8184,10 @@
         <v>767982</v>
       </c>
       <c r="R120" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S120" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
@@ -8231,10 +8231,10 @@
         <v>1779792</v>
       </c>
       <c r="R121" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S121" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
@@ -8278,10 +8278,10 @@
         <v>1779793</v>
       </c>
       <c r="R122" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S122" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="123" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -8325,10 +8325,10 @@
         <v>1779794</v>
       </c>
       <c r="R123" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S123" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
@@ -8372,10 +8372,10 @@
         <v>1779795</v>
       </c>
       <c r="R124" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S124" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
@@ -8419,10 +8419,10 @@
         <v>897535</v>
       </c>
       <c r="R125" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S125" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
@@ -8466,10 +8466,10 @@
         <v>1779796</v>
       </c>
       <c r="R126" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S126" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="127" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -8513,10 +8513,10 @@
         <v>1027616</v>
       </c>
       <c r="R127" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S127" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
@@ -8560,10 +8560,10 @@
         <v>1779797</v>
       </c>
       <c r="R128" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S128" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
@@ -8607,10 +8607,10 @@
         <v>1085497</v>
       </c>
       <c r="R129" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S129" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
@@ -8654,10 +8654,10 @@
         <v>1102857</v>
       </c>
       <c r="R130" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S130" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
@@ -8701,10 +8701,10 @@
         <v>1155107</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S131" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
@@ -8748,10 +8748,10 @@
         <v>1779798</v>
       </c>
       <c r="R132" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S132" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
@@ -8795,10 +8795,10 @@
         <v>1219835</v>
       </c>
       <c r="R133" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S133" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
@@ -8842,10 +8842,10 @@
         <v>1779799</v>
       </c>
       <c r="R134" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S134" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
@@ -8889,10 +8889,10 @@
         <v>1785534</v>
       </c>
       <c r="R135" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S135" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
@@ -8936,10 +8936,10 @@
         <v>1325873</v>
       </c>
       <c r="R136" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S136" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
@@ -8983,10 +8983,10 @@
         <v>1779801</v>
       </c>
       <c r="R137" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S137" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -9030,10 +9030,10 @@
         <v>1455989</v>
       </c>
       <c r="R138" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S138" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
@@ -9077,10 +9077,10 @@
         <v>1779802</v>
       </c>
       <c r="R139" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S139" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
@@ -9124,10 +9124,10 @@
         <v>1779803</v>
       </c>
       <c r="R140" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S140" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
@@ -9171,10 +9171,10 @@
         <v>1779804</v>
       </c>
       <c r="R141" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S141" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
@@ -9218,10 +9218,10 @@
         <v>1779805</v>
       </c>
       <c r="R142" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S142" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
@@ -9265,10 +9265,10 @@
         <v>1779806</v>
       </c>
       <c r="R143" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S143" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
@@ -9312,10 +9312,10 @@
         <v>1779807</v>
       </c>
       <c r="R144" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S144" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
@@ -9359,7 +9359,7 @@
         <v>1785534</v>
       </c>
       <c r="R145" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -9403,7 +9403,7 @@
         <v>1779801</v>
       </c>
       <c r="R146" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
@@ -9447,7 +9447,7 @@
         <v>1779782</v>
       </c>
       <c r="R147" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
@@ -9491,7 +9491,7 @@
         <v>1155107</v>
       </c>
       <c r="R148" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
@@ -9535,7 +9535,7 @@
         <v>1779775</v>
       </c>
       <c r="R149" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="150" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -9579,7 +9579,7 @@
         <v>1779777</v>
       </c>
       <c r="R150" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
@@ -9623,7 +9623,7 @@
         <v>1779778</v>
       </c>
       <c r="R151" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
@@ -9667,7 +9667,7 @@
         <v>1779796</v>
       </c>
       <c r="R152" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
@@ -9711,7 +9711,7 @@
         <v>1779781</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
@@ -9755,7 +9755,7 @@
         <v>1779796</v>
       </c>
       <c r="R154" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
@@ -9799,7 +9799,7 @@
         <v>662849</v>
       </c>
       <c r="R155" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
@@ -9843,7 +9843,7 @@
         <v>1779806</v>
       </c>
       <c r="R156" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
@@ -9851,7 +9851,7 @@
         <v>127</v>
       </c>
       <c r="B157" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C157">
         <v>38.893030400000001</v>
@@ -9887,7 +9887,7 @@
         <v>1702382</v>
       </c>
       <c r="R157" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
@@ -9931,7 +9931,7 @@
         <v>1779797</v>
       </c>
       <c r="R158" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
@@ -9975,7 +9975,7 @@
         <v>1779798</v>
       </c>
       <c r="R159" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
@@ -9983,7 +9983,7 @@
         <v>127</v>
       </c>
       <c r="B160" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C160">
         <v>38.893030400000001</v>
@@ -10019,7 +10019,7 @@
         <v>1702382</v>
       </c>
       <c r="R160" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
@@ -10063,7 +10063,7 @@
         <v>1779796</v>
       </c>
       <c r="R161" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
@@ -10107,7 +10107,7 @@
         <v>1779804</v>
       </c>
       <c r="R162" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>1779786</v>
       </c>
       <c r="R163" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
@@ -10195,7 +10195,7 @@
         <v>1779803</v>
       </c>
       <c r="R164" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>1779798</v>
       </c>
       <c r="R165" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
@@ -10283,7 +10283,7 @@
         <v>606926</v>
       </c>
       <c r="R166" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
@@ -10327,7 +10327,7 @@
         <v>1219835</v>
       </c>
       <c r="R167" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -10341,7 +10341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -10416,10 +10416,10 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -10458,7 +10458,7 @@
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -10497,7 +10497,7 @@
         <v>2080158</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -10536,7 +10536,7 @@
         <v>2614165</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>3</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -10614,7 +10614,7 @@
         <v>4</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -10653,7 +10653,7 @@
         <v>5</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -10692,7 +10692,7 @@
         <v>6</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -10731,7 +10731,7 @@
         <v>6255146</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -10770,7 +10770,7 @@
         <v>6255147</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -10809,7 +10809,7 @@
         <v>6255148</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -10848,7 +10848,7 @@
         <v>6255149</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>6255150</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -10966,7 +10966,7 @@
         <v>6255152</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -11005,7 +11005,7 @@
         <v>6269133</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -11043,7 +11043,7 @@
         <v>6269133</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -11081,7 +11081,7 @@
         <v>6269133</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>6269133</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -11158,7 +11158,7 @@
       </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -11237,7 +11237,7 @@
         <v>6695072</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -11276,7 +11276,7 @@
         <v>6695072</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -11315,7 +11315,7 @@
         <v>6942346</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -11354,7 +11354,7 @@
         <v>7</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -11393,7 +11393,7 @@
         <v>7729882</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -11432,7 +11432,7 @@
         <v>7729883</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>7729891</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -11510,7 +11510,7 @@
         <v>7729900</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -11549,7 +11549,7 @@
         <v>7729901</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -11588,7 +11588,7 @@
         <v>8</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -11627,7 +11627,7 @@
         <v>9</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -11641,8 +11641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11718,15 +11718,15 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B2" t="s">
         <v>379</v>
@@ -11747,10 +11747,10 @@
         <v>379</v>
       </c>
       <c r="H2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I2" t="s">
         <v>409</v>
-      </c>
-      <c r="I2" t="s">
-        <v>410</v>
       </c>
       <c r="J2" t="s">
         <v>378</v>
@@ -11774,12 +11774,12 @@
         <v>10</v>
       </c>
       <c r="R2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>380</v>
@@ -11800,10 +11800,10 @@
         <v>379</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>378</v>
@@ -11828,12 +11828,12 @@
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>381</v>
@@ -11854,10 +11854,10 @@
         <v>379</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>378</v>
@@ -11882,7 +11882,7 @@
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -11929,7 +11929,7 @@
         <v>397</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P5" s="7">
         <v>-1900673</v>
@@ -11938,7 +11938,7 @@
         <v>-2618135</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>397</v>
@@ -11946,7 +11946,7 @@
     </row>
     <row r="6" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>383</v>
@@ -11964,13 +11964,13 @@
         <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>397</v>
@@ -11988,7 +11988,7 @@
         <v>397</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P6" s="7">
         <v>-784547</v>
@@ -11997,7 +11997,7 @@
         <v>-1128888</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>397</v>
@@ -12005,10 +12005,10 @@
     </row>
     <row r="7" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C7" s="6">
         <v>24</v>
@@ -12023,13 +12023,13 @@
         <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>397</v>
@@ -12047,7 +12047,7 @@
         <v>397</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P7" s="7">
         <v>-784547</v>
@@ -12056,7 +12056,7 @@
         <v>-1128888</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>397</v>
@@ -12064,10 +12064,10 @@
     </row>
     <row r="8" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C8" s="6">
         <v>40</v>
@@ -12082,13 +12082,13 @@
         <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>397</v>
@@ -12106,7 +12106,7 @@
         <v>397</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P8" s="7">
         <v>-181585</v>
@@ -12115,15 +12115,15 @@
         <v>-278185</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C9" s="6">
         <v>40</v>
@@ -12138,13 +12138,13 @@
         <v>19</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>397</v>
@@ -12162,7 +12162,7 @@
         <v>397</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P9" s="7">
         <v>-181585</v>
@@ -12171,7 +12171,7 @@
         <v>-278185</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="S9" s="2"/>
     </row>
@@ -12228,8 +12228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:AF1048576"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12304,18 +12304,18 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="C2" s="2">
         <v>19.434170000000002</v>
@@ -12324,22 +12324,22 @@
         <v>-99.13861</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>22</v>
@@ -12348,15 +12348,15 @@
         <v>12</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C3" s="2">
         <v>19.434170000000002</v>
@@ -12365,22 +12365,22 @@
         <v>-99.13861</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>22</v>
@@ -12389,15 +12389,15 @@
         <v>13</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>423</v>
       </c>
       <c r="C4" s="2">
         <v>37</v>
@@ -12415,10 +12415,10 @@
         <v>174</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>22</v>
@@ -12427,15 +12427,15 @@
         <v>14</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C5" s="6">
         <v>31.425070000000002</v>
@@ -12447,16 +12447,16 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>378</v>
@@ -12474,7 +12474,7 @@
         <v>378</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P5" s="7">
         <v>-797156</v>
@@ -12483,7 +12483,7 @@
         <v>-1153429</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -12491,7 +12491,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C6" s="2">
         <v>40.167059999999999</v>
@@ -12530,7 +12530,7 @@
         <v>378</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>432</v>
+        <v>451</v>
       </c>
       <c r="P6" s="7">
         <v>1779795</v>
@@ -12539,15 +12539,15 @@
         <v>378</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C7" s="2">
         <v>40.744819999999997</v>
@@ -12556,10 +12556,10 @@
         <v>-73.948750000000004</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>20</v>
@@ -12574,7 +12574,7 @@
         <v>255</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>378</v>
@@ -12586,7 +12586,7 @@
         <v>378</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>432</v>
+        <v>451</v>
       </c>
       <c r="P7" s="7">
         <v>955863</v>
@@ -12595,15 +12595,15 @@
         <v>378</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C8" s="2">
         <v>40.782589999999999</v>
@@ -12630,7 +12630,7 @@
         <v>289</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>378</v>
@@ -12642,7 +12642,7 @@
         <v>378</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>432</v>
+        <v>451</v>
       </c>
       <c r="P8" s="7">
         <v>1213068</v>
@@ -12651,15 +12651,15 @@
         <v>378</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="C9" s="2">
         <v>31.66667</v>
@@ -12671,16 +12671,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>378</v>
@@ -12698,7 +12698,7 @@
         <v>378</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P9" s="7">
         <v>-793006</v>
@@ -12707,15 +12707,15 @@
         <v>-1144402</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C10" s="2">
         <v>31.66667</v>
@@ -12727,16 +12727,16 @@
         <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>378</v>
@@ -12754,7 +12754,7 @@
         <v>378</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
       <c r="P10" s="7">
         <v>-793006</v>
@@ -12763,7 +12763,7 @@
         <v>-1144402</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted NGA processing to eliminate inconsistent adm1 codes. Removed unneeded step in USGS processing. Cleaned up some minor data errors in adhoc gazetteer.
</commit_message>
<xml_diff>
--- a/GazetteerETL/GeoData/AdHoc/AdHoc.xlsx
+++ b/GazetteerETL/GeoData/AdHoc/AdHoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="15" windowWidth="21720" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="405" yWindow="15" windowWidth="21720" windowHeight="12450" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="USCountry" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2933" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="498">
   <si>
     <t>PLACE_ID</t>
   </si>
@@ -2935,7 +2935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -12854,7 +12854,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12974,9 +12974,6 @@
       <c r="J2" t="s">
         <v>408</v>
       </c>
-      <c r="K2" t="s">
-        <v>377</v>
-      </c>
       <c r="L2" t="s">
         <v>377</v>
       </c>
@@ -13033,9 +13030,6 @@
       <c r="J3" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="L3" s="2" t="s">
         <v>377</v>
       </c>
@@ -13092,9 +13086,6 @@
       </c>
       <c r="J4" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>377</v>
@@ -13495,8 +13486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13745,9 +13736,6 @@
       <c r="J5" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="L5" s="2" t="s">
         <v>377</v>
       </c>
@@ -13981,9 +13969,6 @@
       <c r="J9" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="L9" s="2" t="s">
         <v>377</v>
       </c>
@@ -14039,9 +14024,6 @@
       </c>
       <c r="J10" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>377</v>

</xml_diff>